<commit_message>
Added game project. Added sample sounds. Added FMOD project.
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daifuku\Documents\GitHub\IGME671-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F6133-5B7E-4E38-A96E-A9808AF36B60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1C451-1024-48EC-80FF-3CA7D9D0BF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="5235" windowWidth="21690" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18615" yWindow="1275" windowWidth="15750" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Added game project. Added sample sounds. Added FMOD project."
This reverts commit b8caa8dfcdfbd97b5e16280be0ee879f2050208d.
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daifuku\Documents\GitHub\IGME671-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1C451-1024-48EC-80FF-3CA7D9D0BF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F6133-5B7E-4E38-A96E-A9808AF36B60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18615" yWindow="1275" windowWidth="15750" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="5235" windowWidth="21690" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Created reaper project and started some sound designs.
Added more sound resources.
Updated assets list, including items and status.
Added reaper project with designed sound effects.
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daifuku\Documents\GitHub\IGME671-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3F6133-5B7E-4E38-A96E-A9808AF36B60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B63E1BD-6BEC-43B9-9791-D3C63E3052C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="5235" windowWidth="21690" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15780" yWindow="1815" windowWidth="15750" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Event</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Ambience</t>
   </si>
   <si>
-    <t>White Noise</t>
-  </si>
-  <si>
     <t>Distant Knock Noise 1</t>
   </si>
   <si>
@@ -58,12 +55,6 @@
     <t>Distant Monster Howl 2</t>
   </si>
   <si>
-    <t>Distant Monster Howl 3</t>
-  </si>
-  <si>
-    <t>Distant Monster Howl 4</t>
-  </si>
-  <si>
     <t>Whispers 1</t>
   </si>
   <si>
@@ -91,24 +82,6 @@
     <t>Door Move</t>
   </si>
   <si>
-    <t>Enemy Howl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monster Howl </t>
-  </si>
-  <si>
-    <t>Throat Click</t>
-  </si>
-  <si>
-    <t>Enemy Howl Aggro</t>
-  </si>
-  <si>
-    <t>Monster Howl Aggro</t>
-  </si>
-  <si>
-    <t>Throat Click Aggro</t>
-  </si>
-  <si>
     <t>Player Foot Steps</t>
   </si>
   <si>
@@ -124,34 +97,40 @@
     <t>Foot Step Walk 4</t>
   </si>
   <si>
-    <t>Foot Step Run 1</t>
-  </si>
-  <si>
-    <t>Foot Step Run 2</t>
-  </si>
-  <si>
-    <t>Foot Step Run 3</t>
-  </si>
-  <si>
-    <t>Foot Step Run 4</t>
-  </si>
-  <si>
-    <t>Foot Step Sneak 1</t>
-  </si>
-  <si>
-    <t>Foot Step Sneak 2</t>
-  </si>
-  <si>
-    <t>Foot Step Sneak 3</t>
-  </si>
-  <si>
-    <t>Foot Step Sneak 4</t>
-  </si>
-  <si>
     <t>Push Object</t>
   </si>
   <si>
     <t>Ground Friction Sound</t>
+  </si>
+  <si>
+    <t>Foot Step Walk 5</t>
+  </si>
+  <si>
+    <t>Foot Step Walk 6</t>
+  </si>
+  <si>
+    <t>Reaper</t>
+  </si>
+  <si>
+    <t>White Noise (Loop)</t>
+  </si>
+  <si>
+    <t>Enemy Howl 1</t>
+  </si>
+  <si>
+    <t>Enemy Howl 2</t>
+  </si>
+  <si>
+    <t>Monster Howl 1</t>
+  </si>
+  <si>
+    <t>Monster Howl 2</t>
+  </si>
+  <si>
+    <t>Stress Noise (Loop)</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -422,9 +401,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -454,197 +435,202 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" s="3" t="s">
-        <v>14</v>
+      <c r="D11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="1" t="s">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="1" t="s">
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="C24" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="C25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="C26" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="C27" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="C28" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="C29" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="C30" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="C31" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added friction sound. Implemented friction sound. Updated documentation.
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daifuku\Documents\GitHub\IGME671-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58890222-35CA-4E68-993E-B78CDD92B428}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6907558B-F5B3-401A-9FF6-D372A63B441C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18960" yWindow="4425" windowWidth="19035" windowHeight="16695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="4425" windowWidth="19035" windowHeight="16695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>Event</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Stress Noise (Loop)</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>Recorded</t>
   </si>
   <si>
-    <t>FMOD</t>
-  </si>
-  <si>
     <t>Door Close</t>
   </si>
   <si>
@@ -149,6 +143,9 @@
   </si>
   <si>
     <t>Player Foot Steps (Walk, Run, Sneak)</t>
+  </si>
+  <si>
+    <t>Unity</t>
   </si>
 </sst>
 </file>
@@ -431,7 +428,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -458,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75">
@@ -469,16 +466,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75">
@@ -489,10 +486,10 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75">
@@ -500,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75">
@@ -511,10 +508,10 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75">
@@ -522,10 +519,10 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75">
@@ -533,10 +530,10 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75">
@@ -544,10 +541,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75">
@@ -558,16 +555,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75">
@@ -575,41 +572,41 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75">
       <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75">
@@ -624,10 +621,10 @@
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75">
@@ -642,30 +639,30 @@
         <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75">
@@ -673,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75">
@@ -681,7 +678,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12.75">
@@ -689,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75">
@@ -697,7 +694,7 @@
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75">
@@ -705,15 +702,15 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75">
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75">
@@ -723,15 +720,17 @@
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75"/>

</xml_diff>

<commit_message>
Updated documentation. (I am so sorry, I thought the project is due midnight and I also messed up my time-zone.)
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daifuku\Documents\GitHub\IGME671-Project\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\IGME671-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6907558B-F5B3-401A-9FF6-D372A63B441C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD556D5-965E-41A2-8B31-1A0E1A5B66E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="4425" windowWidth="19035" windowHeight="16695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23" yWindow="630" windowWidth="17971" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>Event</t>
   </si>
@@ -146,6 +146,33 @@
   </si>
   <si>
     <t>Unity</t>
+  </si>
+  <si>
+    <t>Reaper</t>
+  </si>
+  <si>
+    <t>Recorded, enemies are not implemented so not in Unity.</t>
+  </si>
+  <si>
+    <t>UI Hover</t>
+  </si>
+  <si>
+    <t>UI Click</t>
+  </si>
+  <si>
+    <t>UI Drag</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>UI Sound 1</t>
+  </si>
+  <si>
+    <t>UI Sound 2</t>
+  </si>
+  <si>
+    <t>UI Sound 3</t>
   </si>
 </sst>
 </file>
@@ -428,13 +455,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.1328125" customWidth="1"/>
+    <col min="4" max="4" width="24.1328125" customWidth="1"/>
     <col min="6" max="6" width="48" customWidth="1"/>
   </cols>
   <sheetData>
@@ -616,7 +643,9 @@
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
@@ -624,7 +653,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75">
@@ -634,7 +663,9 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
@@ -642,7 +673,7 @@
         <v>34</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75">
@@ -733,9 +764,66 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="12.75"/>
-    <row r="24" spans="1:6" ht="12.75"/>
-    <row r="25" spans="1:6" ht="12.75"/>
+    <row r="23" spans="1:6" ht="12.75">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12.75">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12.75">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1" xr:uid="{C1464BD3-F07B-4F72-BE8A-52912FE29532}"/>

</xml_diff>